<commit_message>
fixed error in heval3
</commit_message>
<xml_diff>
--- a/data/processed/3rd/MASTER_combined_3rd.xlsx
+++ b/data/processed/3rd/MASTER_combined_3rd.xlsx
@@ -9927,7 +9927,7 @@
       </c>
       <c r="T119"/>
       <c r="U119" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="120">
@@ -9990,7 +9990,7 @@
       </c>
       <c r="T120"/>
       <c r="U120" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121">
@@ -10053,7 +10053,7 @@
       </c>
       <c r="T121"/>
       <c r="U121" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122">
@@ -10118,7 +10118,7 @@
         <v>144</v>
       </c>
       <c r="U122" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123">
@@ -10181,7 +10181,7 @@
       </c>
       <c r="T123"/>
       <c r="U123" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="124">
@@ -10244,7 +10244,7 @@
       </c>
       <c r="T124"/>
       <c r="U124" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
     </row>
     <row r="125">
@@ -10309,7 +10309,7 @@
         <v>145</v>
       </c>
       <c r="U125" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
     </row>
     <row r="126">

</xml_diff>